<commit_message>
dotacion en servicio arreglo
</commit_message>
<xml_diff>
--- a/docs/Modelo Relacional.xlsx
+++ b/docs/Modelo Relacional.xlsx
@@ -711,7 +711,7 @@
     <t>ConvencionRestBarCafeteria</t>
   </si>
   <si>
-    <t>idServicioAsignado(ServicioHotelComplementarios.idServicio)</t>
+    <t>idDotacion(Dotacion.idDotacion)</t>
   </si>
 </sst>
 </file>
@@ -941,8 +941,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1079,7 +1081,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1087,6 +1089,7 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1094,6 +1097,7 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1371,7 +1375,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1012"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" zoomScale="125" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A133" zoomScale="135" workbookViewId="0">
       <selection activeCell="D155" sqref="D155"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
consulta 6 pero mal
</commit_message>
<xml_diff>
--- a/docs/Modelo Relacional.xlsx
+++ b/docs/Modelo Relacional.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="415" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="164">
   <si>
     <t>CadenaHotelera</t>
   </si>
@@ -712,6 +712,9 @@
   </si>
   <si>
     <t>idDotacion(Dotacion.idDotacion)</t>
+  </si>
+  <si>
+    <t>cantHabitaciones</t>
   </si>
 </sst>
 </file>
@@ -960,7 +963,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1049,6 +1052,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1375,8 +1387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I1012"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A133" zoomScale="135" workbookViewId="0">
-      <selection activeCell="D155" sqref="D155"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="135" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1394,7 +1406,7 @@
     <col min="11" max="26" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
@@ -1403,7 +1415,7 @@
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1414,7 +1426,7 @@
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
@@ -1425,7 +1437,7 @@
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>5</v>
       </c>
@@ -1436,25 +1448,26 @@
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="28" t="s">
+    <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="29"/>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="29"/>
-      <c r="G6" s="30"/>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="40"/>
+      <c r="C6" s="40"/>
+      <c r="D6" s="40"/>
+      <c r="E6" s="40"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="40"/>
+      <c r="H6" s="40"/>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
@@ -1476,8 +1489,11 @@
       <c r="G7" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H7" s="38" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
         <v>3</v>
       </c>
@@ -1499,8 +1515,11 @@
       <c r="G8" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H8" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>14</v>
       </c>
@@ -1522,15 +1541,18 @@
       <c r="G9" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H9" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="28" t="s">
         <v>18</v>
       </c>
@@ -1539,7 +1561,7 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>19</v>
       </c>
@@ -1552,7 +1574,7 @@
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>3</v>
       </c>
@@ -1565,7 +1587,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>22</v>
       </c>
@@ -1578,14 +1600,14 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="28" t="s">
         <v>24</v>
       </c>
@@ -2931,7 +2953,7 @@
       <c r="D125" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="E125" s="39" t="s">
+      <c r="E125" s="42" t="s">
         <v>139</v>
       </c>
     </row>
@@ -3002,12 +3024,12 @@
     </row>
     <row r="133" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="134" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A134" s="40" t="s">
+      <c r="A134" s="43" t="s">
         <v>145</v>
       </c>
-      <c r="B134" s="41"/>
-      <c r="C134" s="41"/>
-      <c r="D134" s="41"/>
+      <c r="B134" s="44"/>
+      <c r="C134" s="44"/>
+      <c r="D134" s="44"/>
     </row>
     <row r="135" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="25" t="s">
@@ -3019,7 +3041,7 @@
       <c r="C135" s="25" t="s">
         <v>154</v>
       </c>
-      <c r="D135" s="38" t="s">
+      <c r="D135" s="41" t="s">
         <v>157</v>
       </c>
     </row>
@@ -3044,7 +3066,7 @@
       <c r="B137" s="36" t="s">
         <v>112</v>
       </c>
-      <c r="C137" s="45" t="s">
+      <c r="C137" s="48" t="s">
         <v>41</v>
       </c>
       <c r="D137" s="5" t="s">
@@ -3148,52 +3170,52 @@
     </row>
     <row r="153" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="154" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A154" s="42" t="s">
+      <c r="A154" s="45" t="s">
         <v>155</v>
       </c>
-      <c r="B154" s="42"/>
-      <c r="C154" s="42"/>
-      <c r="D154" s="42"/>
+      <c r="B154" s="45"/>
+      <c r="C154" s="45"/>
+      <c r="D154" s="45"/>
     </row>
     <row r="155" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A155" s="43" t="s">
+      <c r="A155" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="B155" s="43" t="s">
+      <c r="B155" s="46" t="s">
         <v>158</v>
       </c>
-      <c r="C155" s="44" t="s">
+      <c r="C155" s="47" t="s">
         <v>159</v>
       </c>
-      <c r="D155" s="45" t="s">
+      <c r="D155" s="48" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="156" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A156" s="46" t="s">
-        <v>3</v>
-      </c>
-      <c r="B156" s="46" t="s">
+      <c r="A156" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="B156" s="49" t="s">
         <v>4</v>
       </c>
-      <c r="C156" s="46" t="s">
-        <v>3</v>
-      </c>
-      <c r="D156" s="46" t="s">
+      <c r="C156" s="49" t="s">
+        <v>3</v>
+      </c>
+      <c r="D156" s="49" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="157" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A157" s="46" t="s">
+      <c r="A157" s="49" t="s">
         <v>112</v>
       </c>
-      <c r="B157" s="47" t="s">
+      <c r="B157" s="50" t="s">
         <v>156</v>
       </c>
-      <c r="C157" s="48" t="s">
+      <c r="C157" s="51" t="s">
         <v>160</v>
       </c>
-      <c r="D157" s="48" t="s">
+      <c r="D157" s="51" t="s">
         <v>160</v>
       </c>
     </row>
@@ -4056,6 +4078,7 @@
   <mergeCells count="32">
     <mergeCell ref="A149:B149"/>
     <mergeCell ref="A36:E36"/>
+    <mergeCell ref="A6:H6"/>
     <mergeCell ref="A134:D134"/>
     <mergeCell ref="A154:D154"/>
     <mergeCell ref="A85:C85"/>
@@ -4080,7 +4103,6 @@
     <mergeCell ref="A11:C11"/>
     <mergeCell ref="A16:E16"/>
     <mergeCell ref="A21:F21"/>
-    <mergeCell ref="A6:G6"/>
     <mergeCell ref="A26:H26"/>
     <mergeCell ref="A76:E76"/>
     <mergeCell ref="A80:G80"/>

</xml_diff>